<commit_message>
Added seeding and helpers. not functional yet. still developing
</commit_message>
<xml_diff>
--- a/SeedingResources/Products.xlsx
+++ b/SeedingResources/Products.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\CyberMuffin\Repos\BlazorEcommerce\SeedingResources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96EE5DD6-A8E2-4B86-8AB2-E591F4A7C820}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D60A876-CCB8-4AB6-8A67-740F6707C7D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3675" yWindow="3675" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,10 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
-  <si>
-    <t>Id</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Title</t>
   </si>
@@ -377,19 +374,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N6" sqref="N6"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="16.28515625" customWidth="1"/>
-    <col min="4" max="4" width="23.85546875" customWidth="1"/>
+    <col min="2" max="2" width="16.28515625" customWidth="1"/>
+    <col min="3" max="3" width="23.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -402,30 +399,24 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2">
+      <c r="D2">
         <v>100</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{81A22B72-B061-4313-A3C9-37637F1ABF14}"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{81A22B72-B061-4313-A3C9-37637F1ABF14}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>

</xml_diff>

<commit_message>
Seeding working correctly. might be able to make it more generic
</commit_message>
<xml_diff>
--- a/SeedingResources/Products.xlsx
+++ b/SeedingResources/Products.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\CyberMuffin\Repos\BlazorEcommerce\SeedingResources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D60A876-CCB8-4AB6-8A67-740F6707C7D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9A28E63-8195-41D3-8958-73D9BCD8CC5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3675" yWindow="3675" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Title</t>
   </si>
@@ -46,6 +46,15 @@
   </si>
   <si>
     <t>www.prod1.com</t>
+  </si>
+  <si>
+    <t>Prod2</t>
+  </si>
+  <si>
+    <t>ProdDesc2</t>
+  </si>
+  <si>
+    <t>www.prod2.com</t>
   </si>
 </sst>
 </file>
@@ -374,10 +383,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -414,11 +423,26 @@
         <v>100</v>
       </c>
     </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3">
+        <v>500</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{81A22B72-B061-4313-A3C9-37637F1ABF14}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{C459BAEC-DC01-4F95-83E8-4D028F8EF39A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
All changes upto the point where I try to remove reflection. might be able to just use generic types
</commit_message>
<xml_diff>
--- a/SeedingResources/Products.xlsx
+++ b/SeedingResources/Products.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\CyberMuffin\Repos\BlazorEcommerce\SeedingResources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9A28E63-8195-41D3-8958-73D9BCD8CC5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDB62983-0333-44D4-943C-7E5011DA5400}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3675" yWindow="3675" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Title</t>
   </si>
@@ -55,6 +55,18 @@
   </si>
   <si>
     <t>www.prod2.com</t>
+  </si>
+  <si>
+    <t>QuantityInStock</t>
+  </si>
+  <si>
+    <t>OnSale</t>
+  </si>
+  <si>
+    <t>True</t>
+  </si>
+  <si>
+    <t>False</t>
   </si>
 </sst>
 </file>
@@ -99,9 +111,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -383,19 +396,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="16.28515625" customWidth="1"/>
     <col min="3" max="3" width="23.85546875" customWidth="1"/>
+    <col min="5" max="5" width="15.85546875" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -408,8 +423,14 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -422,8 +443,14 @@
       <c r="D2">
         <v>100</v>
       </c>
+      <c r="E2">
+        <v>5</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -435,6 +462,12 @@
       </c>
       <c r="D3">
         <v>500</v>
+      </c>
+      <c r="E3">
+        <v>10</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added application configuration and working images from wwwroot
</commit_message>
<xml_diff>
--- a/SeedingResources/Products.xlsx
+++ b/SeedingResources/Products.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\CyberMuffin\Repos\BlazorEcommerce\SeedingResources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDB62983-0333-44D4-943C-7E5011DA5400}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03BC79C2-5B78-4E84-8330-4D564173EAD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3675" yWindow="3675" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -45,18 +45,12 @@
     <t>ProdDesc1</t>
   </si>
   <si>
-    <t>www.prod1.com</t>
-  </si>
-  <si>
     <t>Prod2</t>
   </si>
   <si>
     <t>ProdDesc2</t>
   </si>
   <si>
-    <t>www.prod2.com</t>
-  </si>
-  <si>
     <t>QuantityInStock</t>
   </si>
   <si>
@@ -67,6 +61,12 @@
   </si>
   <si>
     <t>False</t>
+  </si>
+  <si>
+    <t>./images/dota.jpg</t>
+  </si>
+  <si>
+    <t>./images/dotalol.jpg</t>
   </si>
 </sst>
 </file>
@@ -399,7 +399,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -424,10 +424,10 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -438,7 +438,7 @@
         <v>5</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="D2">
         <v>100</v>
@@ -447,18 +447,18 @@
         <v>5</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
         <v>7</v>
       </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
       <c r="C3" s="1" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="D3">
         <v>500</v>
@@ -467,15 +467,11 @@
         <v>10</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{81A22B72-B061-4313-A3C9-37637F1ABF14}"/>
-    <hyperlink ref="C3" r:id="rId2" xr:uid="{C459BAEC-DC01-4F95-83E8-4D028F8EF39A}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
More config changes and seeding
</commit_message>
<xml_diff>
--- a/SeedingResources/Products.xlsx
+++ b/SeedingResources/Products.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\CyberMuffin\Repos\BlazorEcommerce\SeedingResources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07294B79-A1B5-4411-81C6-464DA2F1DED0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A1123F2-844A-4318-87E3-AC0838B42EED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3675" yWindow="3675" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,9 +27,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="208">
   <si>
-    <t>Title</t>
-  </si>
-  <si>
     <t>Description</t>
   </si>
   <si>
@@ -649,6 +646,9 @@
   </si>
   <si>
     <t>ProdDesc99</t>
+  </si>
+  <si>
+    <t>Name</t>
   </si>
 </sst>
 </file>
@@ -987,7 +987,7 @@
   <dimension ref="A1:F100"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+      <selection activeCell="N16" sqref="N16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1000,33 +1000,33 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>207</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
       <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
       <c r="C2" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D2">
         <v>100</v>
@@ -1035,18 +1035,18 @@
         <v>5</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
       <c r="C3" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D3">
         <v>500</v>
@@ -1055,18 +1055,18 @@
         <v>10</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D4">
         <v>900</v>
@@ -1075,18 +1075,18 @@
         <v>15</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D5">
         <v>1300</v>
@@ -1095,18 +1095,18 @@
         <v>20</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D6">
         <v>1700</v>
@@ -1115,18 +1115,18 @@
         <v>25</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D7">
         <v>2100</v>
@@ -1135,18 +1135,18 @@
         <v>30</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B8" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D8">
         <v>2500</v>
@@ -1155,18 +1155,18 @@
         <v>35</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B9" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D9">
         <v>2900</v>
@@ -1175,18 +1175,18 @@
         <v>40</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B10" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D10">
         <v>3300</v>
@@ -1195,18 +1195,18 @@
         <v>45</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B11" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D11">
         <v>3700</v>
@@ -1215,18 +1215,18 @@
         <v>50</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B12" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D12">
         <v>4100</v>
@@ -1235,18 +1235,18 @@
         <v>55</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B13" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D13">
         <v>4500</v>
@@ -1255,18 +1255,18 @@
         <v>60</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B14" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D14">
         <v>4900</v>
@@ -1275,18 +1275,18 @@
         <v>65</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B15" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D15">
         <v>5300</v>
@@ -1295,18 +1295,18 @@
         <v>70</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B16" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D16">
         <v>5700</v>
@@ -1315,18 +1315,18 @@
         <v>75</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B17" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D17">
         <v>6100</v>
@@ -1335,18 +1335,18 @@
         <v>80</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B18" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D18">
         <v>6500</v>
@@ -1355,18 +1355,18 @@
         <v>85</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B19" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D19">
         <v>6900</v>
@@ -1375,18 +1375,18 @@
         <v>90</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B20" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D20">
         <v>7300</v>
@@ -1395,18 +1395,18 @@
         <v>95</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D21">
         <v>7700</v>
@@ -1415,18 +1415,18 @@
         <v>100</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B22" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D22">
         <v>8100</v>
@@ -1435,18 +1435,18 @@
         <v>105</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B23" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D23">
         <v>8500</v>
@@ -1455,18 +1455,18 @@
         <v>110</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B24" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D24">
         <v>8900</v>
@@ -1475,18 +1475,18 @@
         <v>115</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B25" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D25">
         <v>9300</v>
@@ -1495,18 +1495,18 @@
         <v>120</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B26" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D26">
         <v>9700</v>
@@ -1515,18 +1515,18 @@
         <v>125</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B27" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D27">
         <v>10100</v>
@@ -1535,18 +1535,18 @@
         <v>130</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B28" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D28">
         <v>10500</v>
@@ -1555,18 +1555,18 @@
         <v>135</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B29" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D29">
         <v>10900</v>
@@ -1575,18 +1575,18 @@
         <v>140</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B30" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D30">
         <v>11300</v>
@@ -1595,18 +1595,18 @@
         <v>145</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B31" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D31">
         <v>11700</v>
@@ -1615,18 +1615,18 @@
         <v>150</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B32" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D32">
         <v>12100</v>
@@ -1635,18 +1635,18 @@
         <v>155</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B33" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D33">
         <v>12500</v>
@@ -1655,18 +1655,18 @@
         <v>160</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B34" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D34">
         <v>12900</v>
@@ -1675,18 +1675,18 @@
         <v>165</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B35" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D35">
         <v>13300</v>
@@ -1695,18 +1695,18 @@
         <v>170</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B36" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D36">
         <v>13700</v>
@@ -1715,18 +1715,18 @@
         <v>175</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B37" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D37">
         <v>14100</v>
@@ -1735,18 +1735,18 @@
         <v>180</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B38" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D38">
         <v>14500</v>
@@ -1755,18 +1755,18 @@
         <v>185</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B39" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D39">
         <v>14900</v>
@@ -1775,18 +1775,18 @@
         <v>190</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B40" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D40">
         <v>15300</v>
@@ -1795,18 +1795,18 @@
         <v>195</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B41" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D41">
         <v>15700</v>
@@ -1815,18 +1815,18 @@
         <v>200</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B42" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D42">
         <v>16100</v>
@@ -1835,18 +1835,18 @@
         <v>205</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B43" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D43">
         <v>16500</v>
@@ -1855,18 +1855,18 @@
         <v>210</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B44" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D44">
         <v>16900</v>
@@ -1875,18 +1875,18 @@
         <v>215</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B45" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D45">
         <v>17300</v>
@@ -1895,18 +1895,18 @@
         <v>220</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B46" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D46">
         <v>17700</v>
@@ -1915,18 +1915,18 @@
         <v>225</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B47" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D47">
         <v>18100</v>
@@ -1935,18 +1935,18 @@
         <v>230</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B48" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D48">
         <v>18500</v>
@@ -1955,18 +1955,18 @@
         <v>235</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B49" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D49">
         <v>18900</v>
@@ -1975,18 +1975,18 @@
         <v>240</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B50" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D50">
         <v>19300</v>
@@ -1995,18 +1995,18 @@
         <v>245</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B51" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D51">
         <v>19700</v>
@@ -2015,18 +2015,18 @@
         <v>250</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B52" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D52">
         <v>20100</v>
@@ -2035,18 +2035,18 @@
         <v>255</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B53" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D53">
         <v>20500</v>
@@ -2055,18 +2055,18 @@
         <v>260</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B54" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D54">
         <v>20900</v>
@@ -2075,18 +2075,18 @@
         <v>265</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B55" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D55">
         <v>21300</v>
@@ -2095,18 +2095,18 @@
         <v>270</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B56" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D56">
         <v>21700</v>
@@ -2115,18 +2115,18 @@
         <v>275</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B57" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D57">
         <v>22100</v>
@@ -2135,18 +2135,18 @@
         <v>280</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B58" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D58">
         <v>22500</v>
@@ -2155,18 +2155,18 @@
         <v>285</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B59" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D59">
         <v>22900</v>
@@ -2175,18 +2175,18 @@
         <v>290</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B60" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D60">
         <v>23300</v>
@@ -2195,18 +2195,18 @@
         <v>295</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B61" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D61">
         <v>23700</v>
@@ -2215,18 +2215,18 @@
         <v>300</v>
       </c>
       <c r="F61" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B62" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D62">
         <v>24100</v>
@@ -2235,18 +2235,18 @@
         <v>305</v>
       </c>
       <c r="F62" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B63" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D63">
         <v>24500</v>
@@ -2255,18 +2255,18 @@
         <v>310</v>
       </c>
       <c r="F63" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B64" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D64">
         <v>24900</v>
@@ -2275,18 +2275,18 @@
         <v>315</v>
       </c>
       <c r="F64" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B65" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D65">
         <v>25300</v>
@@ -2295,18 +2295,18 @@
         <v>320</v>
       </c>
       <c r="F65" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B66" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D66">
         <v>25700</v>
@@ -2315,18 +2315,18 @@
         <v>325</v>
       </c>
       <c r="F66" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B67" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D67">
         <v>26100</v>
@@ -2335,18 +2335,18 @@
         <v>330</v>
       </c>
       <c r="F67" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B68" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D68">
         <v>26500</v>
@@ -2355,18 +2355,18 @@
         <v>335</v>
       </c>
       <c r="F68" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B69" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D69">
         <v>26900</v>
@@ -2375,18 +2375,18 @@
         <v>340</v>
       </c>
       <c r="F69" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B70" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D70">
         <v>27300</v>
@@ -2395,18 +2395,18 @@
         <v>345</v>
       </c>
       <c r="F70" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B71" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D71">
         <v>27700</v>
@@ -2415,18 +2415,18 @@
         <v>350</v>
       </c>
       <c r="F71" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B72" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D72">
         <v>28100</v>
@@ -2435,18 +2435,18 @@
         <v>355</v>
       </c>
       <c r="F72" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B73" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D73">
         <v>28500</v>
@@ -2455,18 +2455,18 @@
         <v>360</v>
       </c>
       <c r="F73" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B74" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D74">
         <v>28900</v>
@@ -2475,18 +2475,18 @@
         <v>365</v>
       </c>
       <c r="F74" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B75" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D75">
         <v>29300</v>
@@ -2495,18 +2495,18 @@
         <v>370</v>
       </c>
       <c r="F75" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B76" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D76">
         <v>29700</v>
@@ -2515,18 +2515,18 @@
         <v>375</v>
       </c>
       <c r="F76" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B77" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D77">
         <v>30100</v>
@@ -2535,18 +2535,18 @@
         <v>380</v>
       </c>
       <c r="F77" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B78" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D78">
         <v>30500</v>
@@ -2555,18 +2555,18 @@
         <v>385</v>
       </c>
       <c r="F78" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B79" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D79">
         <v>30900</v>
@@ -2575,18 +2575,18 @@
         <v>390</v>
       </c>
       <c r="F79" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B80" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D80">
         <v>31300</v>
@@ -2595,18 +2595,18 @@
         <v>395</v>
       </c>
       <c r="F80" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B81" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D81">
         <v>31700</v>
@@ -2615,18 +2615,18 @@
         <v>400</v>
       </c>
       <c r="F81" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B82" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D82">
         <v>32100</v>
@@ -2635,18 +2635,18 @@
         <v>405</v>
       </c>
       <c r="F82" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B83" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D83">
         <v>32500</v>
@@ -2655,18 +2655,18 @@
         <v>410</v>
       </c>
       <c r="F83" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B84" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D84">
         <v>32900</v>
@@ -2675,18 +2675,18 @@
         <v>415</v>
       </c>
       <c r="F84" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B85" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D85">
         <v>33300</v>
@@ -2695,18 +2695,18 @@
         <v>420</v>
       </c>
       <c r="F85" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B86" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D86">
         <v>33700</v>
@@ -2715,18 +2715,18 @@
         <v>425</v>
       </c>
       <c r="F86" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B87" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D87">
         <v>34100</v>
@@ -2735,18 +2735,18 @@
         <v>430</v>
       </c>
       <c r="F87" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B88" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D88">
         <v>34500</v>
@@ -2755,18 +2755,18 @@
         <v>435</v>
       </c>
       <c r="F88" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B89" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D89">
         <v>34900</v>
@@ -2775,18 +2775,18 @@
         <v>440</v>
       </c>
       <c r="F89" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B90" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D90">
         <v>35300</v>
@@ -2795,18 +2795,18 @@
         <v>445</v>
       </c>
       <c r="F90" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B91" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D91">
         <v>35700</v>
@@ -2815,18 +2815,18 @@
         <v>450</v>
       </c>
       <c r="F91" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B92" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D92">
         <v>36100</v>
@@ -2835,18 +2835,18 @@
         <v>455</v>
       </c>
       <c r="F92" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B93" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D93">
         <v>36500</v>
@@ -2855,18 +2855,18 @@
         <v>460</v>
       </c>
       <c r="F93" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B94" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D94">
         <v>36900</v>
@@ -2875,18 +2875,18 @@
         <v>465</v>
       </c>
       <c r="F94" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B95" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D95">
         <v>37300</v>
@@ -2895,18 +2895,18 @@
         <v>470</v>
       </c>
       <c r="F95" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B96" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D96">
         <v>37700</v>
@@ -2915,18 +2915,18 @@
         <v>475</v>
       </c>
       <c r="F96" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B97" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D97">
         <v>38100</v>
@@ -2935,18 +2935,18 @@
         <v>480</v>
       </c>
       <c r="F97" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B98" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D98">
         <v>38500</v>
@@ -2955,18 +2955,18 @@
         <v>485</v>
       </c>
       <c r="F98" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B99" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D99">
         <v>38900</v>
@@ -2975,18 +2975,18 @@
         <v>490</v>
       </c>
       <c r="F99" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B100" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D100">
         <v>39300</v>
@@ -2995,7 +2995,7 @@
         <v>495</v>
       </c>
       <c r="F100" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>